<commit_message>
update minimal example (besprechung shb jf)
</commit_message>
<xml_diff>
--- a/inst/extdata/example_miss.xlsx
+++ b/inst/extdata/example_miss.xlsx
@@ -47,7 +47,7 @@
     <t xml:space="preserve">sehr gut</t>
   </si>
   <si>
-    <t xml:space="preserve">skala1item1</t>
+    <t xml:space="preserve">skala1_item1</t>
   </si>
   <si>
     <t xml:space="preserve">stimme nicht zu</t>
@@ -62,13 +62,13 @@
     <t xml:space="preserve">stimme voll zu</t>
   </si>
   <si>
-    <t xml:space="preserve">skala1item2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skala1item3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pv_kat1</t>
+    <t xml:space="preserve">skala1_item2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skala1_item3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pvkat_1</t>
   </si>
   <si>
     <t xml:space="preserve">Kompetenzstufe 1</t>
@@ -86,16 +86,16 @@
     <t xml:space="preserve">Kompetenzstufe 5</t>
   </si>
   <si>
-    <t xml:space="preserve">pv_kat2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pv_kat3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pv_kat4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pv_kat5</t>
+    <t xml:space="preserve">pvkat_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pvkat_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pvkat_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pvkat_5</t>
   </si>
   <si>
     <t xml:space="preserve">sf1</t>

</xml_diff>

<commit_message>
start implementing missings in minimal example
</commit_message>
<xml_diff>
--- a/inst/extdata/example_miss.xlsx
+++ b/inst/extdata/example_miss.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">Var.name</t>
   </si>
@@ -29,10 +29,22 @@
     <t xml:space="preserve">Zeilenumbruch_vor_Wert</t>
   </si>
   <si>
+    <t xml:space="preserve">varMetrisch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not reached</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">omission</t>
+  </si>
+  <si>
     <t xml:space="preserve">varOrdinal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nein</t>
   </si>
   <si>
     <t xml:space="preserve">sehr schlecht</t>
@@ -452,7 +464,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>-99</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -461,7 +473,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -469,764 +481,798 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>-98</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B15" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="n">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
       <c r="E17" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
-        <v>19</v>
-      </c>
       <c r="E18" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B21" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E21" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E23" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" t="n">
-        <v>3</v>
-      </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" t="s">
-        <v>21</v>
-      </c>
       <c r="E24" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B25" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B26" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D28" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E28" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B29" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E30" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E31" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="n">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
         <v>25</v>
       </c>
-      <c r="B32" t="n">
-        <v>5</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" t="s">
-        <v>24</v>
-      </c>
       <c r="E32" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="n">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
         <v>26</v>
       </c>
-      <c r="B33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>19</v>
-      </c>
       <c r="E33" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B34" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E34" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E35" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B36" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E36" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B37" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E37" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B38" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E38" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B39" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E39" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B40" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E40" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B41" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E41" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B42" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E42" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B43" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E43" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" t="n">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
         <v>28</v>
       </c>
-      <c r="B44" t="n">
-        <v>2</v>
-      </c>
-      <c r="C44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" t="s">
-        <v>20</v>
-      </c>
       <c r="E44" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B45" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E45" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B46" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E46" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" t="n">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" t="n">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" t="n">
+        <v>5</v>
+      </c>
+      <c r="C49" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" t="s">
         <v>28</v>
       </c>
-      <c r="B47" t="n">
-        <v>5</v>
-      </c>
-      <c r="C47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" t="s">
-        <v>24</v>
-      </c>
-      <c r="E47" t="s">
-        <v>6</v>
+      <c r="E49" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[calculateDescriptives] Fix descriptives for pooled variables
Fix calulcation of descriptives for pooled categorical and nominal variables. Helper functions now mimic behavior and output of functions for not pooled variables.

Also modify example data set to completely cover all different variable types. Adapt tests and resulting example objects accordingly.

#27
</commit_message>
<xml_diff>
--- a/inst/extdata/example_miss.xlsx
+++ b/inst/extdata/example_miss.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">Var.name</t>
   </si>
@@ -80,25 +80,46 @@
     <t xml:space="preserve">skala1_item3</t>
   </si>
   <si>
+    <t xml:space="preserve">pvord_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kompetenzstufe 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kompetenzstufe 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kompetenzstufe 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kompetenzstufe 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pvord_pooled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kompetenzstufe 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pvord_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pvord_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pvord_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pvord_5</t>
+  </si>
+  <si>
     <t xml:space="preserve">pvkat_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Kompetenzstufe 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kompetenzstufe 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kompetenzstufe 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kompetenzstufe 4</t>
-  </si>
-  <si>
     <t xml:space="preserve">pvkat_pooled</t>
   </si>
   <si>
-    <t xml:space="preserve">Kompetenzstufe 5</t>
+    <t xml:space="preserve">Kompetenzstufe 6</t>
   </si>
   <si>
     <t xml:space="preserve">pvkat_2</t>
@@ -1275,6 +1296,618 @@
         <v>8</v>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" t="n">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" t="n">
+        <v>3</v>
+      </c>
+      <c r="C52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" t="s">
+        <v>25</v>
+      </c>
+      <c r="E52" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53" t="n">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" t="s">
+        <v>26</v>
+      </c>
+      <c r="E53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" t="n">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" t="s">
+        <v>23</v>
+      </c>
+      <c r="E55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56" t="n">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" t="s">
+        <v>24</v>
+      </c>
+      <c r="E56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>34</v>
+      </c>
+      <c r="B57" t="n">
+        <v>3</v>
+      </c>
+      <c r="C57" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" t="s">
+        <v>25</v>
+      </c>
+      <c r="E57" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>34</v>
+      </c>
+      <c r="B58" t="n">
+        <v>4</v>
+      </c>
+      <c r="C58" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" t="s">
+        <v>26</v>
+      </c>
+      <c r="E58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>34</v>
+      </c>
+      <c r="B59" t="n">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59" t="s">
+        <v>28</v>
+      </c>
+      <c r="E59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>34</v>
+      </c>
+      <c r="B60" t="n">
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>35</v>
+      </c>
+      <c r="E60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>33</v>
+      </c>
+      <c r="B61" t="n">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" t="s">
+        <v>35</v>
+      </c>
+      <c r="E61" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>36</v>
+      </c>
+      <c r="B62" t="n">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" t="s">
+        <v>23</v>
+      </c>
+      <c r="E62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>36</v>
+      </c>
+      <c r="B63" t="n">
+        <v>2</v>
+      </c>
+      <c r="C63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" t="s">
+        <v>24</v>
+      </c>
+      <c r="E63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>36</v>
+      </c>
+      <c r="B64" t="n">
+        <v>3</v>
+      </c>
+      <c r="C64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" t="s">
+        <v>25</v>
+      </c>
+      <c r="E64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>36</v>
+      </c>
+      <c r="B65" t="n">
+        <v>4</v>
+      </c>
+      <c r="C65" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" t="s">
+        <v>26</v>
+      </c>
+      <c r="E65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>36</v>
+      </c>
+      <c r="B66" t="n">
+        <v>5</v>
+      </c>
+      <c r="C66" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" t="s">
+        <v>28</v>
+      </c>
+      <c r="E66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>36</v>
+      </c>
+      <c r="B67" t="n">
+        <v>6</v>
+      </c>
+      <c r="C67" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" t="s">
+        <v>35</v>
+      </c>
+      <c r="E67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>37</v>
+      </c>
+      <c r="B68" t="n">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" t="s">
+        <v>23</v>
+      </c>
+      <c r="E68" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>37</v>
+      </c>
+      <c r="B69" t="n">
+        <v>2</v>
+      </c>
+      <c r="C69" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" t="s">
+        <v>24</v>
+      </c>
+      <c r="E69" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>37</v>
+      </c>
+      <c r="B70" t="n">
+        <v>3</v>
+      </c>
+      <c r="C70" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" t="s">
+        <v>25</v>
+      </c>
+      <c r="E70" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>37</v>
+      </c>
+      <c r="B71" t="n">
+        <v>4</v>
+      </c>
+      <c r="C71" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" t="s">
+        <v>26</v>
+      </c>
+      <c r="E71" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>37</v>
+      </c>
+      <c r="B72" t="n">
+        <v>5</v>
+      </c>
+      <c r="C72" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" t="s">
+        <v>28</v>
+      </c>
+      <c r="E72" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>37</v>
+      </c>
+      <c r="B73" t="n">
+        <v>6</v>
+      </c>
+      <c r="C73" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" t="s">
+        <v>35</v>
+      </c>
+      <c r="E73" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>38</v>
+      </c>
+      <c r="B74" t="n">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" t="s">
+        <v>23</v>
+      </c>
+      <c r="E74" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>38</v>
+      </c>
+      <c r="B75" t="n">
+        <v>2</v>
+      </c>
+      <c r="C75" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" t="s">
+        <v>24</v>
+      </c>
+      <c r="E75" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>38</v>
+      </c>
+      <c r="B76" t="n">
+        <v>3</v>
+      </c>
+      <c r="C76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" t="s">
+        <v>25</v>
+      </c>
+      <c r="E76" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>38</v>
+      </c>
+      <c r="B77" t="n">
+        <v>4</v>
+      </c>
+      <c r="C77" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" t="s">
+        <v>26</v>
+      </c>
+      <c r="E77" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>38</v>
+      </c>
+      <c r="B78" t="n">
+        <v>5</v>
+      </c>
+      <c r="C78" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" t="s">
+        <v>28</v>
+      </c>
+      <c r="E78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>38</v>
+      </c>
+      <c r="B79" t="n">
+        <v>6</v>
+      </c>
+      <c r="C79" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" t="s">
+        <v>35</v>
+      </c>
+      <c r="E79" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>39</v>
+      </c>
+      <c r="B80" t="n">
+        <v>1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" t="s">
+        <v>23</v>
+      </c>
+      <c r="E80" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>39</v>
+      </c>
+      <c r="B81" t="n">
+        <v>2</v>
+      </c>
+      <c r="C81" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" t="s">
+        <v>24</v>
+      </c>
+      <c r="E81" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>39</v>
+      </c>
+      <c r="B82" t="n">
+        <v>3</v>
+      </c>
+      <c r="C82" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" t="s">
+        <v>25</v>
+      </c>
+      <c r="E82" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>39</v>
+      </c>
+      <c r="B83" t="n">
+        <v>4</v>
+      </c>
+      <c r="C83" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" t="s">
+        <v>26</v>
+      </c>
+      <c r="E83" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>39</v>
+      </c>
+      <c r="B84" t="n">
+        <v>5</v>
+      </c>
+      <c r="C84" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" t="s">
+        <v>28</v>
+      </c>
+      <c r="E84" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>39</v>
+      </c>
+      <c r="B85" t="n">
+        <v>6</v>
+      </c>
+      <c r="C85" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" t="s">
+        <v>35</v>
+      </c>
+      <c r="E85" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>